<commit_message>
Creada la plantilla XML de los pisos
</commit_message>
<xml_diff>
--- a/TonTunaDungeon/src/pisosproyecto.xlsx
+++ b/TonTunaDungeon/src/pisosproyecto.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\NetBeansProjects\TonTuna-Dungeon\TonTunaDungeon\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CFGS\PROGRAMACION\Java\NetBeans\TonTuna-Dungeon\TonTunaDungeon\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Piso1" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -2194,315 +2194,675 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1">
+        <v>61</v>
+      </c>
+      <c r="H1" s="1">
+        <v>71</v>
+      </c>
+      <c r="I1" s="1">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1">
+        <v>91</v>
+      </c>
+      <c r="K1" s="1">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1">
+        <v>41</v>
+      </c>
+      <c r="P1" s="1">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>61</v>
+      </c>
+      <c r="R1" s="1">
+        <v>71</v>
+      </c>
+      <c r="S1" s="1">
+        <v>81</v>
+      </c>
+      <c r="T1" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="T2" s="1"/>
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>92</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="T3" s="1"/>
+      <c r="J3" s="1">
+        <v>93</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="T3" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="4" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
       <c r="C4" s="5"/>
       <c r="F4" s="6"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="T4" s="1"/>
+      <c r="J4" s="1">
+        <v>94</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="T4" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="1">
+        <v>95</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="3"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="5"/>
-      <c r="T5" s="1"/>
+      <c r="T5" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="J6" s="1">
+        <v>96</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6</v>
+      </c>
       <c r="M6" s="5"/>
       <c r="O6" s="2"/>
       <c r="Q6" s="4"/>
-      <c r="T6" s="1"/>
+      <c r="T6" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="G7" s="5"/>
       <c r="H7" s="2"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="J7" s="1">
+        <v>97</v>
+      </c>
+      <c r="K7" s="1">
+        <v>7</v>
+      </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="5"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="2"/>
-      <c r="T7" s="1"/>
+      <c r="T7" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <v>98</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8</v>
+      </c>
+      <c r="T8" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="T9" s="1"/>
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1">
+        <v>99</v>
+      </c>
+      <c r="K9" s="1">
+        <v>9</v>
+      </c>
+      <c r="T9" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1">
+        <v>60</v>
+      </c>
+      <c r="G10" s="1">
+        <v>70</v>
+      </c>
+      <c r="H10" s="1">
+        <v>80</v>
+      </c>
+      <c r="I10" s="1">
+        <v>90</v>
+      </c>
+      <c r="J10" s="1">
+        <v>100</v>
+      </c>
+      <c r="K10" s="1">
+        <v>10</v>
+      </c>
+      <c r="L10" s="1">
+        <v>20</v>
+      </c>
+      <c r="M10" s="1">
+        <v>30</v>
+      </c>
+      <c r="N10" s="1">
+        <v>40</v>
+      </c>
+      <c r="O10" s="1">
+        <v>50</v>
+      </c>
+      <c r="P10" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>70</v>
+      </c>
+      <c r="R10" s="1">
+        <v>80</v>
+      </c>
+      <c r="S10" s="1">
+        <v>90</v>
+      </c>
+      <c r="T10" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1">
+        <v>61</v>
+      </c>
+      <c r="H11" s="1">
+        <v>71</v>
+      </c>
+      <c r="I11" s="1">
+        <v>81</v>
+      </c>
+      <c r="J11" s="1">
+        <v>91</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>11</v>
+      </c>
+      <c r="M11" s="1">
+        <v>21</v>
+      </c>
+      <c r="N11" s="1">
+        <v>31</v>
+      </c>
+      <c r="O11" s="1">
+        <v>41</v>
+      </c>
+      <c r="P11" s="1">
+        <v>51</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>61</v>
+      </c>
+      <c r="R11" s="1">
+        <v>71</v>
+      </c>
+      <c r="S11" s="1">
+        <v>81</v>
+      </c>
+      <c r="T11" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="T12" s="1"/>
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>92</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2</v>
+      </c>
+      <c r="T12" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1">
+        <v>93</v>
+      </c>
+      <c r="K13" s="1">
+        <v>3</v>
+      </c>
       <c r="M13" s="5"/>
       <c r="N13" s="2"/>
       <c r="O13" s="5"/>
-      <c r="T13" s="1"/>
+      <c r="T13" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="5"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="J14" s="1">
+        <v>94</v>
+      </c>
+      <c r="K14" s="1">
+        <v>4</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="T14" s="1"/>
+      <c r="T14" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="G15" s="2"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="1">
+        <v>95</v>
+      </c>
+      <c r="K15" s="1">
+        <v>5</v>
+      </c>
       <c r="L15" s="4"/>
       <c r="M15" s="6"/>
       <c r="O15" s="3"/>
-      <c r="T15" s="1"/>
+      <c r="T15" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>6</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="G16" s="6"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="J16" s="1">
+        <v>96</v>
+      </c>
+      <c r="K16" s="1">
+        <v>6</v>
+      </c>
       <c r="M16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="T16" s="1"/>
+      <c r="T16" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>7</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="J17" s="1">
+        <v>97</v>
+      </c>
+      <c r="K17" s="1">
+        <v>7</v>
+      </c>
       <c r="M17" s="2"/>
       <c r="N17" s="5"/>
       <c r="O17" s="2"/>
-      <c r="T17" s="1"/>
+      <c r="T17" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="T18" s="1"/>
+      <c r="A18" s="1">
+        <v>8</v>
+      </c>
+      <c r="J18" s="1">
+        <v>98</v>
+      </c>
+      <c r="K18" s="1">
+        <v>8</v>
+      </c>
+      <c r="T18" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="T19" s="1"/>
+      <c r="A19" s="1">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1">
+        <v>99</v>
+      </c>
+      <c r="K19" s="1">
+        <v>9</v>
+      </c>
+      <c r="T19" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
+      <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1">
+        <v>60</v>
+      </c>
+      <c r="G20" s="1">
+        <v>70</v>
+      </c>
+      <c r="H20" s="1">
+        <v>80</v>
+      </c>
+      <c r="I20" s="1">
+        <v>90</v>
+      </c>
+      <c r="J20" s="1">
+        <v>100</v>
+      </c>
+      <c r="K20" s="1">
+        <v>10</v>
+      </c>
+      <c r="L20" s="1">
+        <v>20</v>
+      </c>
+      <c r="M20" s="1">
+        <v>30</v>
+      </c>
+      <c r="N20" s="1">
+        <v>40</v>
+      </c>
+      <c r="O20" s="1">
+        <v>50</v>
+      </c>
+      <c r="P20" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>70</v>
+      </c>
+      <c r="R20" s="1">
+        <v>80</v>
+      </c>
+      <c r="S20" s="1">
+        <v>90</v>
+      </c>
+      <c r="T20" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1">
+        <v>31</v>
+      </c>
+      <c r="E21" s="1">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1">
+        <v>51</v>
+      </c>
+      <c r="G21" s="1">
+        <v>61</v>
+      </c>
+      <c r="H21" s="1">
+        <v>71</v>
+      </c>
+      <c r="I21" s="1">
+        <v>81</v>
+      </c>
+      <c r="J21" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <v>3</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="5"/>
       <c r="E23" s="2"/>
       <c r="F23" s="5"/>
       <c r="G23" s="2"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1">
+        <v>4</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="E24" s="2"/>
       <c r="G24" s="6"/>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="E25" s="3"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1">
+        <v>6</v>
+      </c>
       <c r="C26" s="4"/>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
+      <c r="J27" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="A28" s="1">
+        <v>8</v>
+      </c>
+      <c r="J28" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="A29" s="1">
+        <v>9</v>
+      </c>
+      <c r="J29" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="A30" s="1">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1">
+        <v>30</v>
+      </c>
+      <c r="D30" s="1">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1">
+        <v>50</v>
+      </c>
+      <c r="F30" s="1">
+        <v>60</v>
+      </c>
+      <c r="G30" s="1">
+        <v>70</v>
+      </c>
+      <c r="H30" s="1">
+        <v>80</v>
+      </c>
+      <c r="I30" s="1">
+        <v>90</v>
+      </c>
+      <c r="J30" s="1">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2513,321 +2873,681 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1">
+        <v>61</v>
+      </c>
+      <c r="H1" s="1">
+        <v>71</v>
+      </c>
+      <c r="I1" s="1">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1">
+        <v>91</v>
+      </c>
+      <c r="K1" s="1">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1">
+        <v>41</v>
+      </c>
+      <c r="P1" s="1">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>61</v>
+      </c>
+      <c r="R1" s="1">
+        <v>71</v>
+      </c>
+      <c r="S1" s="1">
+        <v>81</v>
+      </c>
+      <c r="T1" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="T2" s="1"/>
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>92</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
       <c r="F3" s="4"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="1">
+        <v>93</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
       <c r="N3" s="2"/>
       <c r="O3" s="5"/>
       <c r="P3" s="2"/>
-      <c r="T3" s="1"/>
+      <c r="T3" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
       <c r="C4" s="2"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="1">
+        <v>94</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="T4" s="1"/>
+      <c r="T4" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="1">
+        <v>95</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" s="3"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="4"/>
-      <c r="T5" s="1"/>
+      <c r="T5" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="F6" s="2"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="J6" s="1">
+        <v>96</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6</v>
+      </c>
       <c r="N6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="T6" s="1"/>
+      <c r="T6" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="5"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="J7" s="1">
+        <v>97</v>
+      </c>
+      <c r="K7" s="1">
+        <v>7</v>
+      </c>
       <c r="N7" s="2"/>
       <c r="O7" s="5"/>
       <c r="P7" s="2"/>
-      <c r="T7" s="1"/>
+      <c r="T7" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <v>98</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8</v>
+      </c>
+      <c r="T8" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="T9" s="1"/>
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1">
+        <v>99</v>
+      </c>
+      <c r="K9" s="1">
+        <v>9</v>
+      </c>
+      <c r="T9" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1">
+        <v>60</v>
+      </c>
+      <c r="G10" s="1">
+        <v>70</v>
+      </c>
+      <c r="H10" s="1">
+        <v>80</v>
+      </c>
+      <c r="I10" s="1">
+        <v>90</v>
+      </c>
+      <c r="J10" s="1">
+        <v>100</v>
+      </c>
+      <c r="K10" s="1">
+        <v>10</v>
+      </c>
+      <c r="L10" s="1">
+        <v>20</v>
+      </c>
+      <c r="M10" s="1">
+        <v>30</v>
+      </c>
+      <c r="N10" s="1">
+        <v>40</v>
+      </c>
+      <c r="O10" s="1">
+        <v>50</v>
+      </c>
+      <c r="P10" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>70</v>
+      </c>
+      <c r="R10" s="1">
+        <v>80</v>
+      </c>
+      <c r="S10" s="1">
+        <v>90</v>
+      </c>
+      <c r="T10" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1">
+        <v>61</v>
+      </c>
+      <c r="H11" s="1">
+        <v>71</v>
+      </c>
+      <c r="I11" s="1">
+        <v>81</v>
+      </c>
+      <c r="J11" s="1">
+        <v>91</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>11</v>
+      </c>
+      <c r="M11" s="1">
+        <v>21</v>
+      </c>
+      <c r="N11" s="1">
+        <v>31</v>
+      </c>
+      <c r="O11" s="1">
+        <v>41</v>
+      </c>
+      <c r="P11" s="1">
+        <v>51</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>61</v>
+      </c>
+      <c r="R11" s="1">
+        <v>71</v>
+      </c>
+      <c r="S11" s="1">
+        <v>81</v>
+      </c>
+      <c r="T11" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="T12" s="1"/>
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>92</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2</v>
+      </c>
+      <c r="T12" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
       <c r="G13" s="2"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="J13" s="1">
+        <v>93</v>
+      </c>
+      <c r="K13" s="1">
+        <v>3</v>
+      </c>
       <c r="O13" s="5"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="T13" s="1"/>
+      <c r="T13" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="J14" s="1">
+        <v>94</v>
+      </c>
+      <c r="K14" s="1">
+        <v>4</v>
+      </c>
       <c r="O14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="T14" s="1"/>
+      <c r="T14" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
       <c r="C15" s="5"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
       <c r="G15" s="5"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="1">
+        <v>95</v>
+      </c>
+      <c r="K15" s="1">
+        <v>5</v>
+      </c>
       <c r="M15" s="5"/>
       <c r="N15" s="2"/>
       <c r="O15" s="3"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="5"/>
-      <c r="T15" s="1"/>
+      <c r="T15" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>6</v>
+      </c>
       <c r="C16" s="2"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="J16" s="1">
+        <v>96</v>
+      </c>
+      <c r="K16" s="1">
+        <v>6</v>
+      </c>
       <c r="O16" s="2"/>
-      <c r="T16" s="1"/>
+      <c r="T16" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>7</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="J17" s="1">
+        <v>97</v>
+      </c>
+      <c r="K17" s="1">
+        <v>7</v>
+      </c>
       <c r="O17" s="2"/>
-      <c r="T17" s="1"/>
+      <c r="T17" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1">
+        <v>8</v>
+      </c>
       <c r="D18" s="5"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="J18" s="1">
+        <v>98</v>
+      </c>
+      <c r="K18" s="1">
+        <v>8</v>
+      </c>
       <c r="O18" s="2"/>
-      <c r="T18" s="1"/>
+      <c r="T18" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="A19" s="1">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1">
+        <v>99</v>
+      </c>
+      <c r="K19" s="1">
+        <v>9</v>
+      </c>
       <c r="O19" s="4"/>
-      <c r="T19" s="1"/>
+      <c r="T19" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
+      <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1">
+        <v>60</v>
+      </c>
+      <c r="G20" s="1">
+        <v>70</v>
+      </c>
+      <c r="H20" s="1">
+        <v>80</v>
+      </c>
+      <c r="I20" s="1">
+        <v>90</v>
+      </c>
+      <c r="J20" s="1">
+        <v>100</v>
+      </c>
+      <c r="K20" s="1">
+        <v>10</v>
+      </c>
+      <c r="L20" s="1">
+        <v>20</v>
+      </c>
+      <c r="M20" s="1">
+        <v>30</v>
+      </c>
+      <c r="N20" s="1">
+        <v>40</v>
+      </c>
+      <c r="O20" s="1">
+        <v>50</v>
+      </c>
+      <c r="P20" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>70</v>
+      </c>
+      <c r="R20" s="1">
+        <v>80</v>
+      </c>
+      <c r="S20" s="1">
+        <v>90</v>
+      </c>
+      <c r="T20" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1">
+        <v>31</v>
+      </c>
+      <c r="E21" s="1">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1">
+        <v>51</v>
+      </c>
+      <c r="G21" s="1">
+        <v>61</v>
+      </c>
+      <c r="H21" s="1">
+        <v>71</v>
+      </c>
+      <c r="I21" s="1">
+        <v>81</v>
+      </c>
+      <c r="J21" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="A23" s="1">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1">
+        <v>4</v>
+      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1">
+        <v>6</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1">
+        <v>8</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="5"/>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1">
+        <v>9</v>
+      </c>
       <c r="E29" s="4"/>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="A30" s="1">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1">
+        <v>30</v>
+      </c>
+      <c r="D30" s="1">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1">
+        <v>50</v>
+      </c>
+      <c r="F30" s="1">
+        <v>60</v>
+      </c>
+      <c r="G30" s="1">
+        <v>70</v>
+      </c>
+      <c r="H30" s="1">
+        <v>80</v>
+      </c>
+      <c r="I30" s="1">
+        <v>90</v>
+      </c>
+      <c r="J30" s="1">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Añadido piso 4 en XML
</commit_message>
<xml_diff>
--- a/TonTunaDungeon/src/pisosproyecto.xlsx
+++ b/TonTunaDungeon/src/pisosproyecto.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>//El tipo de contenido se utiliza con un entero:</t>
   </si>
@@ -530,7 +530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1295,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -1596,22 +1596,20 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" customWidth="1"/>
+    <col min="10" max="11" width="4.5703125" customWidth="1"/>
     <col min="12" max="13" width="5.42578125" customWidth="1"/>
     <col min="14" max="14" width="4.7109375" customWidth="1"/>
     <col min="15" max="15" width="6.42578125" customWidth="1"/>
@@ -2030,6 +2028,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -2038,32 +2037,94 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection sqref="A1:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" customWidth="1"/>
+    <col min="15" max="15" width="5" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="18" max="18" width="5" customWidth="1"/>
+    <col min="19" max="19" width="4.7109375" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>6</v>
+      </c>
+      <c r="R1" s="1">
+        <v>7</v>
+      </c>
+      <c r="S1" s="1">
+        <v>8</v>
+      </c>
+      <c r="T1" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1"/>
@@ -2159,26 +2220,66 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1">
+        <v>9</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2</v>
+      </c>
+      <c r="N11" s="1">
+        <v>3</v>
+      </c>
+      <c r="O11" s="1">
+        <v>4</v>
+      </c>
+      <c r="P11" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>6</v>
+      </c>
+      <c r="R11" s="1">
+        <v>7</v>
+      </c>
+      <c r="S11" s="1">
+        <v>8</v>
+      </c>
+      <c r="T11" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1"/>
@@ -2275,20 +2376,43 @@
       <c r="T20" s="1"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1">
+        <v>7</v>
+      </c>
+      <c r="I21" s="1">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="1"/>
       <c r="J22" s="1"/>
+      <c r="L22" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="1"/>
@@ -2296,11 +2420,17 @@
       <c r="E23" s="5"/>
       <c r="F23" s="2"/>
       <c r="J23" s="1"/>
+      <c r="L23" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="1"/>
       <c r="E24" s="2"/>
       <c r="J24" s="1"/>
+      <c r="L24" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="1"/>
@@ -2311,16 +2441,25 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="J25" s="1"/>
+      <c r="L25" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="1"/>
       <c r="G26" s="5"/>
       <c r="J26" s="1"/>
+      <c r="L26" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="1"/>
       <c r="G27" s="2"/>
       <c r="J27" s="1"/>
+      <c r="L27" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="1"/>
@@ -2351,7 +2490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3031,7 +3170,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K20"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Corregido el piso 1 XML
</commit_message>
<xml_diff>
--- a/TonTunaDungeon/src/pisosproyecto.xlsx
+++ b/TonTunaDungeon/src/pisosproyecto.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="Piso1" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -602,11 +602,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="9" width="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1">
@@ -639,16 +645,36 @@
       <c r="J1" s="1">
         <v>91</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="K1" s="1">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1">
+        <v>41</v>
+      </c>
+      <c r="P1" s="1">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>61</v>
+      </c>
+      <c r="R1" s="1">
+        <v>71</v>
+      </c>
+      <c r="S1" s="1">
+        <v>81</v>
+      </c>
+      <c r="T1" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1">
@@ -657,8 +683,12 @@
       <c r="J2" s="1">
         <v>92</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="T2" s="1"/>
+      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1">
@@ -667,8 +697,12 @@
       <c r="J3" s="1">
         <v>93</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="T3" s="1"/>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="T3" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1">
@@ -677,8 +711,12 @@
       <c r="J4" s="1">
         <v>94</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="T4" s="1"/>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="T4" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1">
@@ -690,10 +728,14 @@
       <c r="J5" s="1">
         <v>95</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
       <c r="O5" s="3"/>
       <c r="P5" s="2"/>
-      <c r="T5" s="1"/>
+      <c r="T5" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="1">
@@ -704,11 +746,15 @@
       <c r="J6" s="1">
         <v>96</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1">
+        <v>6</v>
+      </c>
       <c r="M6" s="4"/>
       <c r="N6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="T6" s="1"/>
+      <c r="T6" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1">
@@ -720,11 +766,15 @@
       <c r="J7" s="1">
         <v>97</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1">
+        <v>7</v>
+      </c>
       <c r="N7" s="2"/>
       <c r="O7" s="5"/>
       <c r="P7" s="2"/>
-      <c r="T7" s="1"/>
+      <c r="T7" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1">
@@ -733,8 +783,12 @@
       <c r="J8" s="1">
         <v>98</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="K8" s="1">
+        <v>8</v>
+      </c>
+      <c r="T8" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="1">
@@ -743,8 +797,12 @@
       <c r="J9" s="1">
         <v>99</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="T9" s="1"/>
+      <c r="K9" s="1">
+        <v>9</v>
+      </c>
+      <c r="T9" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="1">
@@ -777,188 +835,424 @@
       <c r="J10" s="1">
         <v>100</v>
       </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
+      <c r="K10" s="1">
+        <v>10</v>
+      </c>
+      <c r="L10" s="1">
+        <v>20</v>
+      </c>
+      <c r="M10" s="1">
+        <v>30</v>
+      </c>
+      <c r="N10" s="1">
+        <v>40</v>
+      </c>
+      <c r="O10" s="1">
+        <v>50</v>
+      </c>
+      <c r="P10" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>70</v>
+      </c>
+      <c r="R10" s="1">
+        <v>80</v>
+      </c>
+      <c r="S10" s="1">
+        <v>90</v>
+      </c>
+      <c r="T10" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1">
+        <v>61</v>
+      </c>
+      <c r="H11" s="1">
+        <v>71</v>
+      </c>
+      <c r="I11" s="1">
+        <v>81</v>
+      </c>
+      <c r="J11" s="1">
+        <v>91</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>11</v>
+      </c>
+      <c r="M11" s="1">
+        <v>21</v>
+      </c>
+      <c r="N11" s="1">
+        <v>31</v>
+      </c>
+      <c r="O11" s="1">
+        <v>41</v>
+      </c>
+      <c r="P11" s="1">
+        <v>51</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>61</v>
+      </c>
+      <c r="R11" s="1">
+        <v>71</v>
+      </c>
+      <c r="S11" s="1">
+        <v>81</v>
+      </c>
+      <c r="T11" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="T12" s="1"/>
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>92</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2</v>
+      </c>
+      <c r="T12" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="5"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="T13" s="1"/>
+      <c r="J13" s="1">
+        <v>93</v>
+      </c>
+      <c r="K13" s="1">
+        <v>3</v>
+      </c>
+      <c r="T13" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="J14" s="1">
+        <v>94</v>
+      </c>
+      <c r="K14" s="1">
+        <v>4</v>
+      </c>
       <c r="O14" s="2"/>
-      <c r="T14" s="1"/>
+      <c r="T14" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
       <c r="E15" s="3"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="1">
+        <v>95</v>
+      </c>
+      <c r="K15" s="1">
+        <v>5</v>
+      </c>
       <c r="N15" s="5"/>
       <c r="O15" s="3"/>
       <c r="P15" s="2"/>
-      <c r="T15" s="1"/>
+      <c r="T15" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>6</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="J16" s="1">
+        <v>96</v>
+      </c>
+      <c r="K16" s="1">
+        <v>6</v>
+      </c>
       <c r="O16" s="2"/>
-      <c r="T16" s="1"/>
+      <c r="T16" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="A17" s="1">
+        <v>7</v>
+      </c>
+      <c r="J17" s="1">
+        <v>97</v>
+      </c>
+      <c r="K17" s="1">
+        <v>7</v>
+      </c>
       <c r="O17" s="2"/>
-      <c r="T17" s="1"/>
+      <c r="T17" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="A18" s="1">
+        <v>8</v>
+      </c>
+      <c r="J18" s="1">
+        <v>98</v>
+      </c>
+      <c r="K18" s="1">
+        <v>8</v>
+      </c>
       <c r="O18" s="2"/>
-      <c r="T18" s="1"/>
+      <c r="T18" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="A19" s="1">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1">
+        <v>99</v>
+      </c>
+      <c r="K19" s="1">
+        <v>9</v>
+      </c>
       <c r="O19" s="4"/>
-      <c r="T19" s="1"/>
+      <c r="T19" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
+      <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1">
+        <v>60</v>
+      </c>
+      <c r="G20" s="1">
+        <v>70</v>
+      </c>
+      <c r="H20" s="1">
+        <v>80</v>
+      </c>
+      <c r="I20" s="1">
+        <v>90</v>
+      </c>
+      <c r="J20" s="1">
+        <v>100</v>
+      </c>
+      <c r="K20" s="1">
+        <v>10</v>
+      </c>
+      <c r="L20" s="1">
+        <v>20</v>
+      </c>
+      <c r="M20" s="1">
+        <v>30</v>
+      </c>
+      <c r="N20" s="1">
+        <v>40</v>
+      </c>
+      <c r="O20" s="1">
+        <v>50</v>
+      </c>
+      <c r="P20" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>70</v>
+      </c>
+      <c r="R20" s="1">
+        <v>80</v>
+      </c>
+      <c r="S20" s="1">
+        <v>90</v>
+      </c>
+      <c r="T20" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1">
+        <v>31</v>
+      </c>
+      <c r="E21" s="1">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1">
+        <v>51</v>
+      </c>
+      <c r="G21" s="1">
+        <v>61</v>
+      </c>
+      <c r="H21" s="1">
+        <v>71</v>
+      </c>
+      <c r="I21" s="1">
+        <v>81</v>
+      </c>
+      <c r="J21" s="1">
+        <v>91</v>
+      </c>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>92</v>
+      </c>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="A23" s="1">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1">
+        <v>4</v>
+      </c>
       <c r="B24" s="5"/>
       <c r="C24" s="2"/>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
       <c r="B25" s="4"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="3"/>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1">
+        <v>6</v>
+      </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
+      <c r="J27" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="A28" s="1">
+        <v>8</v>
+      </c>
+      <c r="J28" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="A29" s="1">
+        <v>9</v>
+      </c>
+      <c r="J29" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="A30" s="1">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1">
+        <v>30</v>
+      </c>
+      <c r="D30" s="1">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1">
+        <v>50</v>
+      </c>
+      <c r="F30" s="1">
+        <v>60</v>
+      </c>
+      <c r="G30" s="1">
+        <v>70</v>
+      </c>
+      <c r="H30" s="1">
+        <v>80</v>
+      </c>
+      <c r="I30" s="1">
+        <v>90</v>
+      </c>
+      <c r="J30" s="1">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -969,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>

</xml_diff>